<commit_message>
Created company and user schemas, and identified routes for the same
</commit_message>
<xml_diff>
--- a/Strategy_AI_Agent_45_Day_Plan.xlsx
+++ b/Strategy_AI_Agent_45_Day_Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthikvj\Documents\Learning\projects\agent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65082734-7C4F-4DDE-AD66-5E85082F5BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117BBF52-CBA9-4FC5-96DB-E383B73737A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="13380" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="103">
   <si>
     <t>Week</t>
   </si>
@@ -433,7 +433,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -445,13 +445,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -766,7 +759,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,7 +825,9 @@
       <c r="D3" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="7" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -848,7 +843,9 @@
       <c r="D4" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -864,7 +861,9 @@
       <c r="D5" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -880,7 +879,9 @@
       <c r="D6" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="7" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -896,7 +897,9 @@
       <c r="D7" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -912,7 +915,9 @@
       <c r="D8" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="7" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">

</xml_diff>

<commit_message>
Added schemas for objectives and key results
</commit_message>
<xml_diff>
--- a/Strategy_AI_Agent_45_Day_Plan.xlsx
+++ b/Strategy_AI_Agent_45_Day_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthikvj\Documents\Learning\projects\agent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117BBF52-CBA9-4FC5-96DB-E383B73737A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D027739-8991-4AAC-9791-9290AD76F73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="103">
   <si>
     <t>Week</t>
   </si>
@@ -759,7 +759,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,7 +933,9 @@
       <c r="D9" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">

</xml_diff>